<commit_message>
add trace and update training set
</commit_message>
<xml_diff>
--- a/type_of_cancer-含中文名.xlsx
+++ b/type_of_cancer-含中文名.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liujilong\OneDrive\python_code\peafowl\癌种中文名称规范\nnctn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{4A32DC4E-D6C6-4A61-B9C7-2DF9DEA0F928}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{3AFAB450-3333-454B-B9B1-B150D0BFD0ED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8795BE2-EB20-4876-83E1-7239B2B65C65}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15356,7 +15356,7 @@
   </si>
   <si>
     <t>母细胞性浆细胞样树突状细胞瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/2024.html</t>
@@ -15374,14 +15374,14 @@
       </rPr>
       <t>细胞幼淋巴细胞白血病</t>
     </r>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/1233.html</t>
   </si>
   <si>
     <t>基底样阴茎鳞状细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/296.html</t>
@@ -15394,11 +15394,11 @@
   </si>
   <si>
     <t>浸润性乳腺癌（非特指型）</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>乳腺浸润癌（非特指型）</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -15430,25 +15430,25 @@
       </rPr>
       <t>来自于皮肤或者器官</t>
     </r>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>乳腺印戒细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>https://baike.baidu.com/item/%E5%8D%B0%E6%88%92%E7%BB%86%E8%83%9E%E7%99%8C/7812939?fr=aladdin</t>
   </si>
   <si>
     <t>布伦纳肿瘤，良性</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://www.pathologyoutlines.com/topic/ovarytumorb9brenner.html</t>
   </si>
   <si>
     <t>宫颈腺样基底细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/446.html</t>
@@ -15458,61 +15458,61 @@
   </si>
   <si>
     <t>原位结肠腺癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/3349.html</t>
   </si>
   <si>
     <t>卵巢交界性透明细胞肿瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://www.cqvip.com/QK/71983X/201834/7001763835.html</t>
   </si>
   <si>
     <t>透明细胞型室管膜瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/5578.html</t>
   </si>
   <si>
     <t>常规型/经典型脊索瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>软骨样化生癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>肺透明细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>透明细胞型脑膜瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://xueshu.baidu.com/usercenter/paper/show?paperid=dd24352ceba265079deb69ef24915f7e&amp;site=xueshu_se</t>
   </si>
   <si>
     <t>牙源性透明细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://xueshu.baidu.com/usercenter/paper/show?paperid=b36727d488a393faf53509ae9ff0bcf2&amp;site=xueshu_se</t>
   </si>
   <si>
     <t>卵巢透明细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/374.html</t>
   </si>
   <si>
     <t>透明细胞乳头状肾细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://www.wanfangdata.com.cn/details/detail.do?_type=perio&amp;id=zgyszz201710010</t>
@@ -15525,61 +15525,61 @@
   </si>
   <si>
     <t>肾集合管细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>宫颈腺癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/477.html</t>
   </si>
   <si>
     <t>宫颈透明细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/453.html</t>
   </si>
   <si>
     <t>子宫内膜癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>https://baike.baidu.com/item/%E5%AD%90%E5%AE%AB%E5%86%85%E8%86%9C%E7%99%8C/2039?fr=aladdin</t>
   </si>
   <si>
     <t>宫颈毛玻璃样细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>https://baike.baidu.com/item/%E5%AE%AB%E9%A2%88%E6%AF%9B%E7%8E%BB%E7%92%83%E6%A0%B7%E7%BB%86%E8%83%9E%E7%99%8C/15715092?fr=aladdin</t>
   </si>
   <si>
     <t>子宫颈平滑肌肉瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>慢性嗜酸性粒细胞白血病，非特指型</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>https://baike.baidu.com/item/%E6%85%A2%E6%80%A7%E5%97%9C%E9%85%B8%E6%80%A7%E7%B2%92%E7%BB%86%E8%83%9E%E7%99%BD%E8%A1%80%E7%97%85/16812313</t>
   </si>
   <si>
     <t>中肾癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>粘液癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>https://baike.baidu.com/item/%E7%B2%98%E6%B6%B2%E7%99%8C/10973495?fr=aladdin</t>
   </si>
   <si>
     <t>宫颈神经内分泌肿瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>https://wenku.baidu.com/view/51de0e2126284b73f242336c1eb91a37f0113202.html</t>
@@ -15592,7 +15592,7 @@
   </si>
   <si>
     <t>宫颈鳞状细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/438.html</t>
@@ -15608,28 +15608,28 @@
   </si>
   <si>
     <t>软骨母细胞瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/3767.html</t>
   </si>
   <si>
     <t>脊索瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/3728.html</t>
   </si>
   <si>
     <t>第三脑室脊索样胶质瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/5575.html</t>
   </si>
   <si>
     <t>经典霍奇金淋巴瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>移植后淋巴组织增殖性疾病- 经典型霍奇金淋巴瘤型</t>
@@ -15639,35 +15639,35 @@
   </si>
   <si>
     <t>完全性葡萄胎</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>https://baike.baidu.com/item/%E5%AE%8C%E5%85%A8%E6%80%A7%E8%91%A1%E8%90%84%E8%83%8E/15792740?fr=aladdin</t>
   </si>
   <si>
     <t>胆管细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>https://baike.baidu.com/item/%E8%83%86%E7%AE%A1%E7%BB%86%E8%83%9E%E7%99%8C/3677917?fr=aladdin</t>
   </si>
   <si>
     <t>脊索样脑膜瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/5555.html</t>
   </si>
   <si>
     <t>软骨母细胞骨肉瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/1193.html</t>
   </si>
   <si>
     <t>软骨肉瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>https://baike.baidu.com/item/%E8%BD%AF%E9%AA%A8%E8%82%89%E7%98%A4/3583465?fr=aladdin</t>
@@ -15693,14 +15693,14 @@
       </rPr>
       <t>小淋巴细胞淋巴瘤</t>
     </r>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/1242.html</t>
   </si>
   <si>
     <t>小脑脂肪神经细胞瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/5569.html</t>
@@ -15718,22 +15718,22 @@
       </rPr>
       <t>细胞慢性淋巴组织增生性疾病</t>
     </r>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/1291.html</t>
   </si>
   <si>
     <t>结膜黑色素瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>结肠髓样癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>皮肤肥大细胞增多症</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>慢性髓性白血病</t>
@@ -15804,14 +15804,14 @@
   </si>
   <si>
     <t>中枢神经细胞瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/5571.html</t>
   </si>
   <si>
     <t>慢性中性粒细胞白血病</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/3533.html</t>
@@ -15821,7 +15821,7 @@
   </si>
   <si>
     <t>骨化生癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/5573.html</t>
@@ -15831,18 +15831,18 @@
   </si>
   <si>
     <t>脉络丛肿瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>皮肤鳞状细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/909.html</t>
   </si>
   <si>
     <t>细胞神经鞘瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>http://dia.dakapath.com/home/diagnosis/detail/id/592.html</t>
@@ -15900,59 +15900,59 @@
   </si>
   <si>
     <t>Glioma, NOS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">胶质瘤 </t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Gastric Remnant Adenocarcinoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>残胃癌，亦称胃切除术后胃癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Granulosa Cell Tumor</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>颗粒细胞瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Glomangiosarcoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Gliosarcoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Gestational Trophoblastic Disease</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Hepatocellular Carcinoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Histiocytic Dendritic Cell Sarcoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Head and Neck</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Hemangioma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>High-Grade B-Cell Lymphoma, NOS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -15986,7 +15986,7 @@
   </si>
   <si>
     <t>High-Grade B-Cell Lymphoma, with MYC and BCL2 and/or BCL6 Rearrangements</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16077,151 +16077,151 @@
       </rPr>
       <t>重组</t>
     </r>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>High-Grade Endometrial Stromal Sarcoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>High-Grade Glioma, NOS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>High-Grade Neuroendocrine Carcinoma of the Esophagus</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>High-Grade Neuroendocrine Carcinoma of the Stomach</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>胃高级神经内分泌癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>hgonec</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>High-Grade Neuroendocrine Carcinoma of the Ovary</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>high-grade neuroendocrine carcinoma of the ovary</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>LightBlue</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>HGONEC</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>oovc</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>卵巢高级神经内分泌癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>hgsft</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>High-Grade Serous Fallopian Tube Cancer</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>high-grade serous fallopian tube cancer</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>HGSFT</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>高级血清输卵管癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>hgsoc</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>High-Grade Serous Ovarian Cancer</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>high-grade serous ovarian cancer</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>HGSOC</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>soc</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>高级血清卵巢癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>hgsos</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>High-Grade Surface Osteosarcoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>high-grade surface osteosarcoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>White</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>HGSOS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>os</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>高级表面骨肉瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>hhv8dlbcl</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>HHV8 Positive DLBCL, NOS</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>hhv8 positive dlbcl, nos</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>LimeGreen</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>HHV8DLBCL</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>mbn</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16261,62 +16261,62 @@
       </rPr>
       <t>NOS</t>
     </r>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>hl</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Hodgkin Lymphoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>hodgkin lymphoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>HL</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>lnm</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>霍奇金淋巴瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Hemangioblastoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>乳腺来源的乳腺分泌物癌</t>
   </si>
   <si>
     <t>Head and Neck Mucosal Melanoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>头颈部鳞状细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>不明原发性头颈部鳞状细胞癌</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>中枢神经系统血管外皮细胞瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Histiocytic Sarcoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Hepatosplenic T-cell Lymphoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16345,39 +16345,39 @@
   </si>
   <si>
     <t>iampca</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Intestinal Ampullary Carcinoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Inflammatory Breast Cancer</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Intestinal Type Mucinous Carcinoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Breast Invasive Ductal Carcinoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>Interdigitating Dendritic Cell Sarcoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>炎性肌纤维母细胞瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>炎性肌纤维细胞性膀胱肿瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>炎性肌纤维细胞性肺肿瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>导管内乳头状黏液性肿瘤</t>
@@ -16473,19 +16473,19 @@
       </rPr>
       <t>细胞淋巴瘤</t>
     </r>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>朗格罕氏细胞组织细胞病</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>朗格罕氏细胞肉瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>低级中央骨肉瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16499,31 +16499,31 @@
       </rPr>
       <t>NOS</t>
     </r>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>低级血清卵巢癌</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hepatoblastoma</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>liver</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>淋巴血清淋巴瘤</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>原发性不明癌</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
-    <t>低级血清卵巢癌</t>
+    <t>分化型脊索瘤</t>
     <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hepatoblastoma</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>liver</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>淋巴血清淋巴瘤</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>原发性不明癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>分化型脊索瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16561,15 +16561,15 @@
   </si>
   <si>
     <t>婴儿星形细胞瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>婴儿促纤维增生型神经节细胞胶质瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>扩散型内因性脑桥神经胶质瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16589,7 +16589,7 @@
       </rPr>
       <t>与慢性炎症</t>
     </r>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16649,11 +16649,11 @@
   </si>
   <si>
     <t>纤维增生性小圆细胞瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>结缔组织增生性毛发上皮瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16718,7 +16718,7 @@
       </rPr>
       <t>细胞淋巴瘤</t>
     </r>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16741,7 +16741,7 @@
   </si>
   <si>
     <t>子宫颈腺癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16764,15 +16764,15 @@
       </rPr>
       <t>切斯特病/脂质肉芽肿病</t>
     </r>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>上皮样血管内皮细胞瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>肝外胆管癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16795,19 +16795,19 @@
       </rPr>
       <t>淋巴瘤）</t>
     </r>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>胚胎性癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>分泌粘蛋白的汗腺癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>囊性胶质瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16839,11 +16839,11 @@
   </si>
   <si>
     <t>胚胎型横纹肌肉瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>富含神经胶质和真玫瑰花结的胚胎性肿瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16875,11 +16875,11 @@
   </si>
   <si>
     <t>多花性滤泡增生</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>FH缺乏性肾细胞癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16911,15 +16911,15 @@
   </si>
   <si>
     <t>成胶质细胞瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>胆囊腺癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>多形恶性神经胶质瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -16998,31 +16998,31 @@
   </si>
   <si>
     <t>胃肠基底细胞癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>成神经节细胞瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>神经节神经胶质瘤</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>尿道鳞状细胞癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>乳腺癌</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>骨癌</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
-    <t>骨癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
     <t>肠癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -17045,74 +17045,70 @@
       </rPr>
       <t>脑癌</t>
     </r>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
-    <t>子宫颈癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>眼睛癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>肾癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>肝癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>头颈癌</t>
   </si>
   <si>
     <t>肺癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>淋巴癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>髓癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>卵巢癌/输卵管癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>胰腺癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>阴茎癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>腹膜癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>胸膜癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>周围神经系统癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>前列腺癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>皮肤癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>软组织癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -17134,39 +17130,39 @@
       </rPr>
       <t>胃癌</t>
     </r>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>睾丸癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>胸腺癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>甲状腺癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>子宫癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>阴道癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>壶腹癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>肾上腺癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>胆道癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -17188,30 +17184,41 @@
       </rPr>
       <t>尿路癌</t>
     </r>
-    <phoneticPr fontId="14" type="noConversion"/>
+    <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
     <t>结直肠癌</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>结肠癌</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>直肠癌</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
-    <t>结肠癌</t>
+    <t>宫颈癌</t>
     <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>直肠癌</t>
-    <phoneticPr fontId="14" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -17376,38 +17383,41 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -17719,10 +17729,10 @@
   <dimension ref="A1:I855"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G660" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G153" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G670" sqref="G670"/>
+      <selection pane="bottomRight" activeCell="G163" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -18170,7 +18180,7 @@
         <v>118</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>4275</v>
+        <v>4274</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -18998,7 +19008,7 @@
         <v>118</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>4274</v>
+        <v>4273</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -19826,7 +19836,7 @@
         <v>118</v>
       </c>
       <c r="G91" s="14" t="s">
-        <v>4276</v>
+        <v>4275</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -19918,7 +19928,7 @@
         <v>118</v>
       </c>
       <c r="G95" s="14" t="s">
-        <v>4277</v>
+        <v>4276</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -21588,7 +21598,7 @@
         <v>118</v>
       </c>
       <c r="G163" s="15" t="s">
-        <v>4251</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -22341,7 +22351,7 @@
         <v>722</v>
       </c>
       <c r="G193" s="14" t="s">
-        <v>4279</v>
+        <v>4278</v>
       </c>
       <c r="H193" s="13" t="s">
         <v>4086</v>
@@ -22367,7 +22377,7 @@
         <v>139</v>
       </c>
       <c r="G194" s="14" t="s">
-        <v>4278</v>
+        <v>4277</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -24081,7 +24091,7 @@
         <v>118</v>
       </c>
       <c r="G268" s="15" t="s">
-        <v>4252</v>
+        <v>4251</v>
       </c>
     </row>
     <row r="269" spans="1:7">
@@ -25116,7 +25126,7 @@
         <v>118</v>
       </c>
       <c r="G313" s="14" t="s">
-        <v>4255</v>
+        <v>4254</v>
       </c>
     </row>
     <row r="314" spans="1:7">
@@ -26404,7 +26414,7 @@
         <v>118</v>
       </c>
       <c r="G369" s="15" t="s">
-        <v>4253</v>
+        <v>4252</v>
       </c>
     </row>
     <row r="370" spans="1:7">
@@ -26956,7 +26966,7 @@
         <v>118</v>
       </c>
       <c r="G393" s="15" t="s">
-        <v>4254</v>
+        <v>4253</v>
       </c>
     </row>
     <row r="394" spans="1:7">
@@ -27232,7 +27242,7 @@
         <v>118</v>
       </c>
       <c r="G405" s="15" t="s">
-        <v>4256</v>
+        <v>4255</v>
       </c>
     </row>
     <row r="406" spans="1:7">
@@ -27347,7 +27357,7 @@
         <v>118</v>
       </c>
       <c r="G410" s="14" t="s">
-        <v>4257</v>
+        <v>4256</v>
       </c>
     </row>
     <row r="411" spans="1:7">
@@ -29785,7 +29795,7 @@
         <v>118</v>
       </c>
       <c r="G516" s="23" t="s">
-        <v>4258</v>
+        <v>4257</v>
       </c>
     </row>
     <row r="517" spans="1:7">
@@ -30957,8 +30967,8 @@
       <c r="F567" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="G567" s="23" t="s">
-        <v>4259</v>
+      <c r="G567" s="24" t="s">
+        <v>4258</v>
       </c>
     </row>
     <row r="568" spans="1:7">
@@ -31142,7 +31152,7 @@
         <v>118</v>
       </c>
       <c r="G575" s="23" t="s">
-        <v>4260</v>
+        <v>4259</v>
       </c>
     </row>
     <row r="576" spans="1:7">
@@ -31763,7 +31773,7 @@
         <v>118</v>
       </c>
       <c r="G602" s="15" t="s">
-        <v>4261</v>
+        <v>4260</v>
       </c>
     </row>
     <row r="603" spans="1:7">
@@ -31809,7 +31819,7 @@
         <v>118</v>
       </c>
       <c r="G604" s="14" t="s">
-        <v>4262</v>
+        <v>4261</v>
       </c>
     </row>
     <row r="605" spans="1:7">
@@ -32108,7 +32118,7 @@
         <v>118</v>
       </c>
       <c r="G617" s="15" t="s">
-        <v>4263</v>
+        <v>4262</v>
       </c>
     </row>
     <row r="618" spans="1:7">
@@ -32384,7 +32394,7 @@
         <v>118</v>
       </c>
       <c r="G629" s="14" t="s">
-        <v>4264</v>
+        <v>4263</v>
       </c>
     </row>
     <row r="630" spans="1:7">
@@ -32660,7 +32670,7 @@
         <v>118</v>
       </c>
       <c r="G641" s="15" t="s">
-        <v>4265</v>
+        <v>4264</v>
       </c>
     </row>
     <row r="642" spans="1:7">
@@ -33327,7 +33337,7 @@
         <v>722</v>
       </c>
       <c r="G670" s="14" t="s">
-        <v>4280</v>
+        <v>4279</v>
       </c>
     </row>
     <row r="671" spans="1:7">
@@ -34569,7 +34579,7 @@
         <v>118</v>
       </c>
       <c r="G724" s="15" t="s">
-        <v>4266</v>
+        <v>4265</v>
       </c>
     </row>
     <row r="725" spans="1:7">
@@ -34845,7 +34855,7 @@
         <v>118</v>
       </c>
       <c r="G736" s="15" t="s">
-        <v>4267</v>
+        <v>4266</v>
       </c>
     </row>
     <row r="737" spans="1:7">
@@ -35282,7 +35292,7 @@
         <v>118</v>
       </c>
       <c r="G755" s="15" t="s">
-        <v>4268</v>
+        <v>4267</v>
       </c>
     </row>
     <row r="756" spans="1:7">
@@ -35512,7 +35522,7 @@
         <v>118</v>
       </c>
       <c r="G765" s="15" t="s">
-        <v>4269</v>
+        <v>4268</v>
       </c>
     </row>
     <row r="766" spans="1:7">
@@ -35788,7 +35798,7 @@
         <v>118</v>
       </c>
       <c r="G777" s="15" t="s">
-        <v>4270</v>
+        <v>4269</v>
       </c>
     </row>
     <row r="778" spans="1:7">
@@ -35811,7 +35821,7 @@
         <v>118</v>
       </c>
       <c r="G778" s="15" t="s">
-        <v>4271</v>
+        <v>4270</v>
       </c>
     </row>
     <row r="779" spans="1:7" s="2" customFormat="1">
@@ -37007,7 +37017,7 @@
         <v>118</v>
       </c>
       <c r="G830" s="15" t="s">
-        <v>4272</v>
+        <v>4271</v>
       </c>
     </row>
     <row r="831" spans="1:7">
@@ -37421,7 +37431,7 @@
         <v>118</v>
       </c>
       <c r="G848" s="15" t="s">
-        <v>4273</v>
+        <v>4272</v>
       </c>
     </row>
     <row r="849" spans="1:7">
@@ -37586,7 +37596,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <conditionalFormatting sqref="G530">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>

</xml_diff>